<commit_message>
added new sheet for stacked pcb
</commit_message>
<xml_diff>
--- a/i2C Materialliste/Elektronik.xlsx
+++ b/i2C Materialliste/Elektronik.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jan\Documents\github\fiberprinter-electronics\i2C Materialliste\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64213D71-D36E-4909-B20B-2AE24949E305}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93B9C0EE-2218-4E67-AFC0-D0AB8C7A7026}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="57840" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28695" yWindow="0" windowWidth="29010" windowHeight="15585" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DifI2C" sheetId="5" r:id="rId1"/>
@@ -1611,6 +1611,12 @@
     <xf numFmtId="164" fontId="1" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="165" fontId="0" fillId="8" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1634,12 +1640,6 @@
     </xf>
     <xf numFmtId="165" fontId="3" fillId="9" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2602,7 +2602,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="Y25" sqref="Y25"/>
+      <selection pane="bottomLeft" activeCell="K27" sqref="K27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2680,18 +2680,18 @@
       <c r="R1" t="s">
         <v>16</v>
       </c>
-      <c r="S1" s="57" t="s">
+      <c r="S1" s="59" t="s">
         <v>180</v>
       </c>
-      <c r="T1" s="58"/>
+      <c r="T1" s="60"/>
       <c r="U1" s="37">
         <f>SUMIFS(N6:N38,O6:O38, "Nicht Gekauft",P6:P38,"Benötigt")</f>
         <v>83</v>
       </c>
-      <c r="W1" s="55" t="s">
+      <c r="W1" s="57" t="s">
         <v>181</v>
       </c>
-      <c r="X1" s="56"/>
+      <c r="X1" s="58"/>
       <c r="Y1" s="26">
         <f>SUM(N2:N38)</f>
         <v>243.05999999999995</v>
@@ -3108,11 +3108,11 @@
       <c r="M10" s="13">
         <v>1</v>
       </c>
-      <c r="N10" s="63">
+      <c r="N10" s="55">
         <f>L10*M10</f>
         <v>8.0500000000000007</v>
       </c>
-      <c r="O10" s="64"/>
+      <c r="O10" s="56"/>
       <c r="P10" s="6"/>
     </row>
     <row r="11" spans="1:25" x14ac:dyDescent="0.25">
@@ -3203,7 +3203,7 @@
         <f t="shared" ref="N12" si="2">L12*M12</f>
         <v>0.78</v>
       </c>
-      <c r="O12" s="64"/>
+      <c r="O12" s="56"/>
       <c r="P12" s="6"/>
       <c r="Q12" s="24"/>
     </row>
@@ -4475,10 +4475,10 @@
         <f>SUBTOTAL(9,F1:F38)</f>
         <v>0.112465</v>
       </c>
-      <c r="L40" s="61" t="s">
+      <c r="L40" s="63" t="s">
         <v>294</v>
       </c>
-      <c r="M40" s="62"/>
+      <c r="M40" s="64"/>
       <c r="N40" s="39">
         <f>SUBTOTAL(9,N1:N38)</f>
         <v>177.14</v>
@@ -4489,10 +4489,10 @@
     </row>
     <row r="43" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G43" s="7"/>
-      <c r="L43" s="59" t="s">
+      <c r="L43" s="61" t="s">
         <v>293</v>
       </c>
-      <c r="M43" s="60"/>
+      <c r="M43" s="62"/>
       <c r="N43" s="25">
         <f>SUBTOTAL(9,R1:R38)</f>
         <v>100.82999999999998</v>

</xml_diff>

<commit_message>
made first pcb design of module 1 with components on front and back
</commit_message>
<xml_diff>
--- a/i2C Materialliste/Elektronik.xlsx
+++ b/i2C Materialliste/Elektronik.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jan\Documents\github\fiberprinter-electronics\i2C Materialliste\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93B9C0EE-2218-4E67-AFC0-D0AB8C7A7026}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{325C240B-A1A4-43BA-8D6C-AB99E8EA218F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28695" yWindow="0" windowWidth="29010" windowHeight="15585" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="10824" yWindow="12852" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DifI2C" sheetId="5" r:id="rId1"/>
@@ -2256,6 +2256,7 @@
         <filter val="B1"/>
         <filter val="B2"/>
         <filter val="B3"/>
+        <filter val="K1"/>
         <filter val="K2"/>
         <filter val="SR2"/>
         <filter val="TP1"/>
@@ -2602,7 +2603,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K27" sqref="K27"/>
+      <selection pane="bottomLeft" activeCell="K17" sqref="K17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3504,7 +3505,7 @@
         <v>1.32</v>
       </c>
     </row>
-    <row r="19" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A19" s="45" t="s">
         <v>132</v>
       </c>
@@ -4481,7 +4482,7 @@
       <c r="M40" s="64"/>
       <c r="N40" s="39">
         <f>SUBTOTAL(9,N1:N38)</f>
-        <v>177.14</v>
+        <v>189.16</v>
       </c>
     </row>
     <row r="42" spans="1:18" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
rearanged the text for module 3
</commit_message>
<xml_diff>
--- a/i2C Materialliste/Elektronik.xlsx
+++ b/i2C Materialliste/Elektronik.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jan\Documents\github\fiberprinter-electronics\i2C Materialliste\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{325C240B-A1A4-43BA-8D6C-AB99E8EA218F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FF28D82-CB4E-4ED9-8F2A-2ED06AE1840D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10824" yWindow="12852" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DifI2C" sheetId="5" r:id="rId1"/>
@@ -2603,7 +2603,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K17" sqref="K17"/>
+      <selection pane="bottomLeft" activeCell="T28" sqref="T27:U28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
added imported components, changed structure
</commit_message>
<xml_diff>
--- a/i2C Materialliste/Elektronik.xlsx
+++ b/i2C Materialliste/Elektronik.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jan\Documents\github\fiberprinter-electronics\i2C Materialliste\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FF28D82-CB4E-4ED9-8F2A-2ED06AE1840D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4444BDB-5EAC-4A73-8B48-96241F734B8E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38280" yWindow="2880" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DifI2C" sheetId="5" r:id="rId1"/>
@@ -2603,7 +2603,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="T28" sqref="T27:U28"/>
+      <selection pane="bottomLeft" activeCell="D43" sqref="D43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>